<commit_message>
Tentativa de correção de encoding
</commit_message>
<xml_diff>
--- a/v2022/dados/dados-originais/setores_analise_conferencia.xlsx
+++ b/v2022/dados/dados-originais/setores_analise_conferencia.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{D06C6E4C-1201-4B63-A419-FBD08C131A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos" sheetId="27" r:id="rId1"/>
@@ -25304,7 +25304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF52446C-9EF4-4110-AF02-A7517D72778D}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -25669,7 +25669,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J3" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29863,7 +29863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEE39C-C79C-4AA3-9576-586312CED21A}">
   <dimension ref="A1:W284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>

</xml_diff>